<commit_message>
Update ke hoach làm việc
</commit_message>
<xml_diff>
--- a/ProjectPlan.xlsx
+++ b/ProjectPlan.xlsx
@@ -253,11 +253,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -542,7 +542,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,14 +554,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -599,7 +599,7 @@
       <c r="E3" s="2">
         <v>5</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -619,7 +619,7 @@
       <c r="E4" s="2">
         <v>4</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -639,7 +639,7 @@
       <c r="E5" s="2">
         <v>5</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -659,7 +659,7 @@
       <c r="E6" s="2">
         <v>7</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -679,8 +679,8 @@
       <c r="E7" s="2">
         <v>1</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>39</v>
+      <c r="F7" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update ke hoach lam viec
</commit_message>
<xml_diff>
--- a/ProjectPlan.xlsx
+++ b/ProjectPlan.xlsx
@@ -542,7 +542,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F6" sqref="F6:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,8 +679,8 @@
       <c r="E7" s="2">
         <v>1</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>36</v>
+      <c r="F7" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>